<commit_message>
ultimos cambios con enrichment.
</commit_message>
<xml_diff>
--- a/BA_events_testMnew.xlsx
+++ b/BA_events_testMnew.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Resumen" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">CONC!$A$1:$N$101</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">CONC!$A$1:$O$101</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="113">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -63,6 +63,9 @@
     <t xml:space="preserve">Origen</t>
   </si>
   <si>
+    <t xml:space="preserve">OrigenTag</t>
+  </si>
+  <si>
     <t xml:space="preserve">Observaciones</t>
   </si>
   <si>
@@ -88,6 +91,9 @@
   </si>
   <si>
     <t xml:space="preserve">Regional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOL/BRA/PAR</t>
   </si>
   <si>
     <t xml:space="preserve">SC</t>
@@ -120,6 +126,9 @@
     <t xml:space="preserve">Mesopotamia</t>
   </si>
   <si>
+    <t xml:space="preserve">MES (ARG)</t>
+  </si>
+  <si>
     <t xml:space="preserve">DN</t>
   </si>
   <si>
@@ -147,6 +156,9 @@
     <t xml:space="preserve">incendio amazonas</t>
   </si>
   <si>
+    <t xml:space="preserve">BOL/BRA/PAR/MES</t>
+  </si>
+  <si>
     <t xml:space="preserve">Datos del Observador 4 – cambiar no por SO</t>
   </si>
   <si>
@@ -162,10 +174,16 @@
     <t xml:space="preserve">Bs. As.</t>
   </si>
   <si>
+    <t xml:space="preserve">BA (ARG)</t>
+  </si>
+  <si>
     <t xml:space="preserve">SL</t>
   </si>
   <si>
     <t xml:space="preserve">Chile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL</t>
   </si>
   <si>
     <t xml:space="preserve">Bs. as.</t>
@@ -184,6 +202,9 @@
   </si>
   <si>
     <t xml:space="preserve">fuegos en australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUS</t>
   </si>
   <si>
     <t xml:space="preserve">AUSTRALIA/CHILE/NEUQUEN/BSAS</t>
@@ -734,15 +755,15 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1000"/>
+  <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K72" activeCellId="0" sqref="K72"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="M88" activeCellId="0" sqref="M88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.8125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="15.14"/>
@@ -751,7 +772,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="33.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="39.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="39.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,8 +815,11 @@
       <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" s="9" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,22 +839,23 @@
         <v>0.509858807017544</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
-      <c r="N2" s="9" t="n">
+      <c r="N2" s="8"/>
+      <c r="O2" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -851,22 +876,23 @@
         <v>0.499241586956522</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="9" t="n">
+      <c r="N3" s="8"/>
+      <c r="O3" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -887,22 +913,23 @@
         <v>0.7347548</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
-      <c r="N4" s="9" t="n">
+      <c r="N4" s="8"/>
+      <c r="O4" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -923,22 +950,23 @@
         <v>1.19260968316832</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
-      <c r="N5" s="9" t="n">
+      <c r="N5" s="8"/>
+      <c r="O5" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -959,22 +987,23 @@
         <v>0.43373725</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
-      <c r="N6" s="9" t="n">
+      <c r="N6" s="8"/>
+      <c r="O6" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -995,22 +1024,23 @@
         <v>1.03454433333333</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
-      <c r="N7" s="9" t="n">
+      <c r="N7" s="8"/>
+      <c r="O7" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1031,22 +1061,23 @@
         <v>1.0762931</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
-      <c r="N8" s="9" t="n">
+      <c r="N8" s="8"/>
+      <c r="O8" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1067,22 +1098,23 @@
         <v>1.0368655</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
-      <c r="N9" s="9" t="n">
+      <c r="N9" s="8"/>
+      <c r="O9" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1103,22 +1135,23 @@
         <v>0.510182083333333</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
-      <c r="N10" s="9" t="n">
+      <c r="N10" s="8"/>
+      <c r="O10" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1139,22 +1172,23 @@
         <v>0.628600555555556</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
-      <c r="N11" s="9" t="n">
+      <c r="N11" s="8"/>
+      <c r="O11" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1175,22 +1209,23 @@
         <v>0.702352763888889</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
-      <c r="N12" s="9" t="n">
+      <c r="N12" s="8"/>
+      <c r="O12" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1211,22 +1246,23 @@
         <v>0.842384479452055</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
-      <c r="N13" s="9" t="n">
+      <c r="N13" s="8"/>
+      <c r="O13" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1247,22 +1283,23 @@
         <v>1.17002332352941</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
-      <c r="N14" s="9" t="n">
+      <c r="N14" s="8"/>
+      <c r="O14" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1283,22 +1320,23 @@
         <v>0.247635011560694</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
-      <c r="N15" s="9" t="n">
+      <c r="N15" s="8"/>
+      <c r="O15" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1319,22 +1357,23 @@
         <v>1.05060265217391</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
-      <c r="N16" s="9" t="n">
+      <c r="N16" s="8"/>
+      <c r="O16" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1355,22 +1394,23 @@
         <v>1.06950337704918</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
-      <c r="N17" s="9" t="n">
+      <c r="N17" s="8"/>
+      <c r="O17" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1391,24 +1431,27 @@
         <v>0.878866545905707</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="13" t="n">
+      <c r="M18" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="12"/>
+      <c r="O18" s="13" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1425,22 +1468,23 @@
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
-      <c r="N19" s="13" t="n">
+      <c r="N19" s="12"/>
+      <c r="O19" s="13" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1461,22 +1505,23 @@
         <v>1.50325183333333</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
-      <c r="N20" s="9" t="n">
+      <c r="N20" s="8"/>
+      <c r="O20" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1494,10 +1539,10 @@
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
       <c r="G21" s="16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I21" s="16" t="str">
         <f aca="false">G21</f>
@@ -1507,7 +1552,8 @@
       <c r="K21" s="16"/>
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
-      <c r="N21" s="17" t="n">
+      <c r="N21" s="16"/>
+      <c r="O21" s="17" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1525,19 +1571,20 @@
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
-      <c r="N22" s="9" t="n">
+      <c r="N22" s="8"/>
+      <c r="O22" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1555,10 +1602,10 @@
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
       <c r="G23" s="16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I23" s="16" t="str">
         <f aca="false">G23</f>
@@ -1568,7 +1615,8 @@
       <c r="K23" s="16"/>
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
-      <c r="N23" s="17" t="n">
+      <c r="N23" s="16"/>
+      <c r="O23" s="17" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1590,10 +1638,10 @@
       </c>
       <c r="F24" s="16"/>
       <c r="G24" s="16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I24" s="16" t="str">
         <f aca="false">G24</f>
@@ -1603,7 +1651,8 @@
       <c r="K24" s="16"/>
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
-      <c r="N24" s="17" t="n">
+      <c r="N24" s="16"/>
+      <c r="O24" s="17" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1620,22 +1669,23 @@
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
-      <c r="N25" s="13" t="n">
+      <c r="N25" s="12"/>
+      <c r="O25" s="13" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1653,10 +1703,10 @@
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
       <c r="G26" s="16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I26" s="16" t="str">
         <f aca="false">G26</f>
@@ -1666,7 +1716,8 @@
       <c r="K26" s="16"/>
       <c r="L26" s="16"/>
       <c r="M26" s="16"/>
-      <c r="N26" s="17" t="n">
+      <c r="N26" s="16"/>
+      <c r="O26" s="17" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1684,19 +1735,20 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H27" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
-      <c r="N27" s="9" t="n">
+      <c r="N27" s="8"/>
+      <c r="O27" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1717,22 +1769,23 @@
         <v>1.24706230612245</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H28" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
-      <c r="N28" s="9" t="n">
+      <c r="N28" s="8"/>
+      <c r="O28" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1749,22 +1802,23 @@
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
       <c r="M29" s="12"/>
-      <c r="N29" s="13" t="n">
+      <c r="N29" s="12"/>
+      <c r="O29" s="13" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1785,26 +1839,27 @@
         <v>1.25022511111111</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M30" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="N30" s="13" t="n">
+        <v>30</v>
+      </c>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="O30" s="13" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1825,22 +1880,23 @@
         <v>1.57611228571429</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H31" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
-      <c r="N31" s="9" t="n">
+      <c r="N31" s="8"/>
+      <c r="O31" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1857,26 +1913,31 @@
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="13" t="n">
+        <v>32</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="N32" s="12"/>
+      <c r="O32" s="13" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1894,10 +1955,10 @@
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
       <c r="G33" s="16" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I33" s="16" t="str">
         <f aca="false">G33</f>
@@ -1907,7 +1968,8 @@
       <c r="K33" s="16"/>
       <c r="L33" s="16"/>
       <c r="M33" s="16"/>
-      <c r="N33" s="17" t="n">
+      <c r="N33" s="16"/>
+      <c r="O33" s="17" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1925,19 +1987,20 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
-      <c r="N34" s="9" t="n">
+      <c r="N34" s="8"/>
+      <c r="O34" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1958,22 +2021,23 @@
         <v>1.212169</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H35" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
-      <c r="N35" s="9" t="n">
+      <c r="N35" s="8"/>
+      <c r="O35" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1994,22 +2058,23 @@
         <v>0.43259440625</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H36" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
-      <c r="N36" s="9" t="n">
+      <c r="N36" s="8"/>
+      <c r="O36" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2030,22 +2095,23 @@
         <v>0.981173706349207</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H37" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
-      <c r="N37" s="9" t="n">
+      <c r="N37" s="8"/>
+      <c r="O37" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2066,28 +2132,31 @@
         <v>1.2788452962963</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L38" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="M38" s="12"/>
-      <c r="N38" s="13" t="n">
+        <v>35</v>
+      </c>
+      <c r="M38" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N38" s="12"/>
+      <c r="O38" s="13" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2108,24 +2177,25 @@
         <v>0.891150205479452</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H39" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I39" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
-      <c r="M39" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="N39" s="9" t="n">
+      <c r="M39" s="8"/>
+      <c r="N39" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O39" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2146,24 +2216,25 @@
         <v>1.02793206896552</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H40" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I40" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
-      <c r="M40" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="N40" s="9" t="n">
+      <c r="M40" s="8"/>
+      <c r="N40" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O40" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2184,28 +2255,31 @@
         <v>1.383551</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L41" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="M41" s="12"/>
-      <c r="N41" s="13" t="n">
+        <v>35</v>
+      </c>
+      <c r="M41" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N41" s="12"/>
+      <c r="O41" s="13" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2226,28 +2300,31 @@
         <v>0.86211475</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I42" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="L42" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="M42" s="12"/>
-      <c r="N42" s="13" t="n">
+        <v>35</v>
+      </c>
+      <c r="M42" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N42" s="12"/>
+      <c r="O42" s="13" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2268,30 +2345,33 @@
         <v>1.46733505633803</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J43" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="L43" s="12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="M43" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="N43" s="13" t="n">
+        <v>22</v>
+      </c>
+      <c r="N43" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="O43" s="13" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2312,30 +2392,33 @@
         <v>1.516236</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="M44" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="N44" s="13" t="n">
+        <v>22</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="O44" s="13" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2352,28 +2435,31 @@
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I45" s="12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J45" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K45" s="12"/>
       <c r="L45" s="12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="M45" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="N45" s="13" t="n">
+        <v>22</v>
+      </c>
+      <c r="N45" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="O45" s="13" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2394,22 +2480,23 @@
         <v>1.1401608137931</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H46" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I46" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="M46" s="8"/>
-      <c r="N46" s="9" t="n">
+      <c r="N46" s="8"/>
+      <c r="O46" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2430,22 +2517,23 @@
         <v>0.688018344827586</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H47" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I47" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J47" s="8"/>
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
       <c r="M47" s="8"/>
-      <c r="N47" s="9" t="n">
+      <c r="N47" s="8"/>
+      <c r="O47" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2462,26 +2550,29 @@
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J48" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K48" s="12"/>
       <c r="L48" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="M48" s="12"/>
-      <c r="N48" s="13" t="n">
+        <v>35</v>
+      </c>
+      <c r="M48" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N48" s="12"/>
+      <c r="O48" s="13" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2498,26 +2589,29 @@
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J49" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K49" s="12"/>
       <c r="L49" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="M49" s="12"/>
-      <c r="N49" s="13" t="n">
+        <v>35</v>
+      </c>
+      <c r="M49" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N49" s="12"/>
+      <c r="O49" s="13" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2538,22 +2632,23 @@
         <v>1.26060492763158</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H50" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I50" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
-      <c r="N50" s="9" t="n">
+      <c r="N50" s="8"/>
+      <c r="O50" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2574,28 +2669,31 @@
         <v>1.72430663076923</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J51" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K51" s="12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L51" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="M51" s="12"/>
-      <c r="N51" s="13" t="n">
+        <v>35</v>
+      </c>
+      <c r="M51" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N51" s="12"/>
+      <c r="O51" s="13" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2616,26 +2714,29 @@
         <v>0.966215441860465</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H52" s="18" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="I52" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J52" s="18"/>
       <c r="K52" s="18"/>
       <c r="L52" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M52" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="N52" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="N52" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="O52" s="0" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2656,24 +2757,25 @@
         <v>0.600562924731183</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H53" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I53" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
-      <c r="M53" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="N53" s="9" t="n">
+      <c r="M53" s="8"/>
+      <c r="N53" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="O53" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2694,22 +2796,23 @@
         <v>0.983993447368421</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H54" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I54" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J54" s="8"/>
       <c r="K54" s="8"/>
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
-      <c r="N54" s="9" t="n">
+      <c r="N54" s="8"/>
+      <c r="O54" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2730,26 +2833,29 @@
         <v>1.046564</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G55" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H55" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I55" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H55" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I55" s="12" t="s">
-        <v>16</v>
-      </c>
       <c r="J55" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K55" s="12"/>
       <c r="L55" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="M55" s="12"/>
-      <c r="N55" s="13" t="n">
+        <v>35</v>
+      </c>
+      <c r="M55" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N55" s="12"/>
+      <c r="O55" s="13" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2770,28 +2876,31 @@
         <v>1.73953896774194</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G56" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H56" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I56" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J56" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L56" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="M56" s="12"/>
-      <c r="N56" s="13" t="n">
+        <v>35</v>
+      </c>
+      <c r="M56" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N56" s="12"/>
+      <c r="O56" s="13" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2809,19 +2918,20 @@
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H57" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I57" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J57" s="8"/>
       <c r="K57" s="8"/>
       <c r="L57" s="8"/>
       <c r="M57" s="8"/>
-      <c r="N57" s="9" t="n">
+      <c r="N57" s="8"/>
+      <c r="O57" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2842,22 +2952,23 @@
         <v>1.43679937951807</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H58" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I58" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J58" s="8"/>
       <c r="K58" s="8"/>
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
-      <c r="N58" s="9" t="n">
+      <c r="N58" s="8"/>
+      <c r="O58" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2878,26 +2989,29 @@
         <v>1.02183162962963</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G59" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H59" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I59" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="H59" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="I59" s="12" t="s">
-        <v>16</v>
       </c>
       <c r="J59" s="12" t="s">
         <v>9</v>
       </c>
       <c r="K59" s="12"/>
       <c r="L59" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="M59" s="12"/>
-      <c r="N59" s="13" t="n">
+        <v>48</v>
+      </c>
+      <c r="M59" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N59" s="12"/>
+      <c r="O59" s="13" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2915,19 +3029,20 @@
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H60" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I60" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J60" s="8"/>
       <c r="K60" s="8"/>
       <c r="L60" s="8"/>
       <c r="M60" s="8"/>
-      <c r="N60" s="9" t="n">
+      <c r="N60" s="8"/>
+      <c r="O60" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2948,22 +3063,23 @@
         <v>0.961475944099378</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H61" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I61" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J61" s="8"/>
       <c r="K61" s="8"/>
       <c r="L61" s="8"/>
       <c r="M61" s="8"/>
-      <c r="N61" s="9" t="n">
+      <c r="N61" s="8"/>
+      <c r="O61" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2984,28 +3100,31 @@
         <v>1.23781</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H62" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J62" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K62" s="12" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="L62" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="M62" s="12"/>
-      <c r="N62" s="13" t="n">
+        <v>51</v>
+      </c>
+      <c r="M62" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N62" s="12"/>
+      <c r="O62" s="13" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3026,22 +3145,23 @@
         <v>0.770984827338129</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H63" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I63" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
       <c r="L63" s="8"/>
       <c r="M63" s="8"/>
-      <c r="N63" s="9" t="n">
+      <c r="N63" s="8"/>
+      <c r="O63" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3059,19 +3179,20 @@
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H64" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I64" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J64" s="8"/>
       <c r="K64" s="8"/>
       <c r="L64" s="8"/>
       <c r="M64" s="8"/>
-      <c r="N64" s="9" t="n">
+      <c r="N64" s="8"/>
+      <c r="O64" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3092,22 +3213,23 @@
         <v>0.900937777777778</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H65" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I65" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I65" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J65" s="8"/>
       <c r="K65" s="8"/>
       <c r="L65" s="8"/>
       <c r="M65" s="8"/>
-      <c r="N65" s="9" t="n">
+      <c r="N65" s="8"/>
+      <c r="O65" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3128,22 +3250,23 @@
         <v>0.772298905660378</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H66" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J66" s="12"/>
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
       <c r="M66" s="12"/>
-      <c r="N66" s="13" t="n">
+      <c r="N66" s="12"/>
+      <c r="O66" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3164,22 +3287,23 @@
         <v>0.642724304347826</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H67" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I67" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I67" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J67" s="8"/>
       <c r="K67" s="8"/>
       <c r="L67" s="8"/>
       <c r="M67" s="8"/>
-      <c r="N67" s="9" t="n">
+      <c r="N67" s="8"/>
+      <c r="O67" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3200,28 +3324,31 @@
         <v>1.21729356521739</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G68" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H68" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J68" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K68" s="12" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="L68" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="M68" s="12"/>
-      <c r="N68" s="13" t="n">
+        <v>51</v>
+      </c>
+      <c r="M68" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N68" s="12"/>
+      <c r="O68" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3242,22 +3369,23 @@
         <v>1.03860773529412</v>
       </c>
       <c r="F69" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G69" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H69" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I69" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J69" s="12"/>
       <c r="K69" s="12"/>
       <c r="L69" s="12"/>
       <c r="M69" s="12"/>
-      <c r="N69" s="13" t="n">
+      <c r="N69" s="12"/>
+      <c r="O69" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3278,28 +3406,31 @@
         <v>1.27146304375</v>
       </c>
       <c r="F70" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H70" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I70" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J70" s="12" t="s">
         <v>9</v>
       </c>
       <c r="K70" s="12" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="L70" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="M70" s="12"/>
-      <c r="N70" s="13" t="n">
+        <v>48</v>
+      </c>
+      <c r="M70" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N70" s="12"/>
+      <c r="O70" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3320,22 +3451,23 @@
         <v>1.29882684615385</v>
       </c>
       <c r="F71" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G71" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H71" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I71" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J71" s="12"/>
       <c r="K71" s="12"/>
       <c r="L71" s="12"/>
       <c r="M71" s="12"/>
-      <c r="N71" s="13" t="n">
+      <c r="N71" s="12"/>
+      <c r="O71" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3356,28 +3488,31 @@
         <v>1.16579975886525</v>
       </c>
       <c r="F72" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G72" s="12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H72" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I72" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J72" s="12" t="s">
         <v>9</v>
       </c>
       <c r="K72" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L72" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="M72" s="12"/>
-      <c r="N72" s="13" t="n">
+        <v>32</v>
+      </c>
+      <c r="M72" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="N72" s="12"/>
+      <c r="O72" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3398,22 +3533,23 @@
         <v>0.526924511450382</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H73" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I73" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I73" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J73" s="8"/>
       <c r="K73" s="8"/>
       <c r="L73" s="8"/>
       <c r="M73" s="8"/>
-      <c r="N73" s="9" t="n">
+      <c r="N73" s="8"/>
+      <c r="O73" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3434,22 +3570,23 @@
         <v>1.15243975</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H74" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I74" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I74" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J74" s="8"/>
       <c r="K74" s="8"/>
       <c r="L74" s="8"/>
       <c r="M74" s="8"/>
-      <c r="N74" s="9" t="n">
+      <c r="N74" s="8"/>
+      <c r="O74" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3470,22 +3607,23 @@
         <v>1.01949652380952</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H75" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I75" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I75" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J75" s="8"/>
       <c r="K75" s="8"/>
       <c r="L75" s="8"/>
       <c r="M75" s="8"/>
-      <c r="N75" s="9" t="n">
+      <c r="N75" s="8"/>
+      <c r="O75" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3506,22 +3644,23 @@
         <v>1.03208732620321</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H76" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I76" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I76" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J76" s="8"/>
       <c r="K76" s="8"/>
       <c r="L76" s="8"/>
       <c r="M76" s="8"/>
-      <c r="N76" s="9" t="n">
+      <c r="N76" s="8"/>
+      <c r="O76" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3542,22 +3681,23 @@
         <v>1.01991402649007</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H77" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I77" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I77" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J77" s="8"/>
       <c r="K77" s="8"/>
       <c r="L77" s="8"/>
       <c r="M77" s="8"/>
-      <c r="N77" s="9" t="n">
+      <c r="N77" s="8"/>
+      <c r="O77" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3578,22 +3718,23 @@
         <v>1.02417112658228</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G78" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H78" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I78" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I78" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J78" s="8"/>
       <c r="K78" s="8"/>
       <c r="L78" s="8"/>
       <c r="M78" s="8"/>
-      <c r="N78" s="9" t="n">
+      <c r="N78" s="8"/>
+      <c r="O78" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3614,28 +3755,31 @@
         <v>1.08134336666667</v>
       </c>
       <c r="F79" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G79" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H79" s="12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I79" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J79" s="13" t="s">
         <v>9</v>
       </c>
       <c r="K79" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L79" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="M79" s="12"/>
-      <c r="N79" s="13" t="n">
+        <v>32</v>
+      </c>
+      <c r="M79" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="N79" s="12"/>
+      <c r="O79" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3656,22 +3800,23 @@
         <v>0.877221</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H80" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I80" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J80" s="8"/>
       <c r="K80" s="8"/>
       <c r="L80" s="8"/>
       <c r="M80" s="8"/>
-      <c r="N80" s="9" t="n">
+      <c r="N80" s="8"/>
+      <c r="O80" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3692,22 +3837,23 @@
         <v>1.30902159134615</v>
       </c>
       <c r="F81" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H81" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I81" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I81" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J81" s="8"/>
       <c r="K81" s="8"/>
       <c r="L81" s="8"/>
       <c r="M81" s="8"/>
-      <c r="N81" s="9" t="n">
+      <c r="N81" s="8"/>
+      <c r="O81" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3724,22 +3870,23 @@
       <c r="D82" s="8"/>
       <c r="E82" s="8"/>
       <c r="F82" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H82" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I82" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I82" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J82" s="8"/>
       <c r="K82" s="8"/>
       <c r="L82" s="8"/>
       <c r="M82" s="8"/>
-      <c r="N82" s="9" t="n">
+      <c r="N82" s="8"/>
+      <c r="O82" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3760,26 +3907,29 @@
         <v>0.7380234</v>
       </c>
       <c r="F83" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G83" s="12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H83" s="12" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="I83" s="12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J83" s="12" t="s">
         <v>9</v>
       </c>
       <c r="K83" s="12"/>
       <c r="L83" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="M83" s="12"/>
-      <c r="N83" s="13" t="n">
+        <v>48</v>
+      </c>
+      <c r="M83" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N83" s="12"/>
+      <c r="O83" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3800,26 +3950,27 @@
         <v>0.652622229508197</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H84" s="8" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="I84" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J84" s="8"/>
       <c r="K84" s="8"/>
       <c r="L84" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="M84" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N84" s="9" t="n">
+        <v>57</v>
+      </c>
+      <c r="M84" s="8"/>
+      <c r="N84" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O84" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3840,28 +3991,31 @@
         <v>1.06957197222222</v>
       </c>
       <c r="F85" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G85" s="12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H85" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I85" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J85" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K85" s="8"/>
       <c r="L85" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="M85" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="N85" s="13" t="n">
+        <v>57</v>
+      </c>
+      <c r="M85" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N85" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="O85" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3882,28 +4036,31 @@
         <v>1.05013729761905</v>
       </c>
       <c r="F86" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G86" s="12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H86" s="12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I86" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J86" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K86" s="8"/>
       <c r="L86" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="M86" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="N86" s="13" t="n">
+        <v>57</v>
+      </c>
+      <c r="M86" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N86" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="O86" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3924,28 +4081,31 @@
         <v>1.43357752820513</v>
       </c>
       <c r="F87" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G87" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H87" s="12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I87" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J87" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K87" s="8"/>
       <c r="L87" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="M87" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="N87" s="13" t="n">
+        <v>57</v>
+      </c>
+      <c r="M87" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N87" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="O87" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3966,26 +4126,29 @@
         <v>1.18826742857143</v>
       </c>
       <c r="F88" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G88" s="12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H88" s="12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I88" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J88" s="12" t="s">
         <v>9</v>
       </c>
       <c r="K88" s="12"/>
       <c r="L88" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="M88" s="12"/>
-      <c r="N88" s="13" t="n">
+        <v>48</v>
+      </c>
+      <c r="M88" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N88" s="12"/>
+      <c r="O88" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -4006,26 +4169,29 @@
         <v>1.11060859259259</v>
       </c>
       <c r="F89" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G89" s="12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H89" s="12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I89" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J89" s="12" t="s">
         <v>9</v>
       </c>
       <c r="K89" s="12"/>
       <c r="L89" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="M89" s="12"/>
-      <c r="N89" s="13" t="n">
+        <v>48</v>
+      </c>
+      <c r="M89" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N89" s="12"/>
+      <c r="O89" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -4046,28 +4212,31 @@
         <v>0.913923494186046</v>
       </c>
       <c r="F90" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G90" s="12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H90" s="12" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="I90" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J90" s="12" t="s">
         <v>9</v>
       </c>
       <c r="K90" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L90" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="M90" s="12"/>
-      <c r="N90" s="13" t="n">
+        <v>62</v>
+      </c>
+      <c r="M90" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="N90" s="12"/>
+      <c r="O90" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -4085,19 +4254,20 @@
       <c r="E91" s="16"/>
       <c r="F91" s="16"/>
       <c r="G91" s="16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H91" s="16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I91" s="16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J91" s="16"/>
       <c r="K91" s="16"/>
       <c r="L91" s="16"/>
       <c r="M91" s="16"/>
-      <c r="N91" s="17" t="n">
+      <c r="N91" s="16"/>
+      <c r="O91" s="17" t="n">
         <v>23</v>
       </c>
     </row>
@@ -4118,28 +4288,31 @@
         <v>0.983014304694423</v>
       </c>
       <c r="F92" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G92" s="12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H92" s="12" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="I92" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J92" s="12" t="s">
         <v>9</v>
       </c>
       <c r="K92" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L92" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="M92" s="12"/>
-      <c r="N92" s="13" t="n">
+        <v>32</v>
+      </c>
+      <c r="M92" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="N92" s="12"/>
+      <c r="O92" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -4160,22 +4333,23 @@
         <v>0.987089936893204</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G93" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H93" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I93" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I93" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J93" s="8"/>
       <c r="K93" s="8"/>
       <c r="L93" s="8"/>
       <c r="M93" s="8"/>
-      <c r="N93" s="9" t="n">
+      <c r="N93" s="8"/>
+      <c r="O93" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -4196,28 +4370,31 @@
         <v>0.959812181478016</v>
       </c>
       <c r="F94" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G94" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H94" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I94" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J94" s="12" t="s">
         <v>9</v>
       </c>
       <c r="K94" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L94" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="M94" s="12"/>
-      <c r="N94" s="13" t="n">
+        <v>32</v>
+      </c>
+      <c r="M94" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="N94" s="12"/>
+      <c r="O94" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -4238,22 +4415,23 @@
         <v>0.787264</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G95" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H95" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I95" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I95" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J95" s="8"/>
       <c r="K95" s="8"/>
       <c r="L95" s="8"/>
       <c r="M95" s="8"/>
-      <c r="N95" s="9" t="n">
+      <c r="N95" s="8"/>
+      <c r="O95" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -4274,22 +4452,23 @@
         <v>1.14074691752577</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H96" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I96" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I96" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J96" s="8"/>
       <c r="K96" s="8"/>
       <c r="L96" s="8"/>
       <c r="M96" s="8"/>
-      <c r="N96" s="9" t="n">
+      <c r="N96" s="8"/>
+      <c r="O96" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -4310,22 +4489,23 @@
         <v>0.781452411764706</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H97" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I97" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I97" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J97" s="8"/>
       <c r="K97" s="8"/>
       <c r="L97" s="8"/>
       <c r="M97" s="8"/>
-      <c r="N97" s="9" t="n">
+      <c r="N97" s="8"/>
+      <c r="O97" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -4346,22 +4526,23 @@
         <v>0.44478180952381</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G98" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H98" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I98" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I98" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="J98" s="8"/>
       <c r="K98" s="8"/>
       <c r="L98" s="8"/>
       <c r="M98" s="8"/>
-      <c r="N98" s="9" t="n">
+      <c r="N98" s="8"/>
+      <c r="O98" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -4382,22 +4563,23 @@
         <v>1.23533518699187</v>
       </c>
       <c r="F99" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G99" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H99" s="12" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="I99" s="12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J99" s="12"/>
       <c r="K99" s="12"/>
       <c r="L99" s="12"/>
       <c r="M99" s="12"/>
-      <c r="N99" s="13" t="n">
+      <c r="N99" s="12"/>
+      <c r="O99" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -4415,19 +4597,20 @@
       <c r="E100" s="16"/>
       <c r="F100" s="16"/>
       <c r="G100" s="16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H100" s="16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I100" s="16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J100" s="16"/>
       <c r="K100" s="16"/>
       <c r="L100" s="16"/>
       <c r="M100" s="16"/>
-      <c r="N100" s="17" t="n">
+      <c r="N100" s="16"/>
+      <c r="O100" s="17" t="n">
         <v>23</v>
       </c>
     </row>
@@ -4448,22 +4631,23 @@
         <v>1.17759195402299</v>
       </c>
       <c r="F101" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G101" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H101" s="12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I101" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J101" s="12"/>
       <c r="K101" s="12"/>
       <c r="L101" s="12"/>
       <c r="M101" s="12"/>
-      <c r="N101" s="13" t="n">
+      <c r="N101" s="12"/>
+      <c r="O101" s="13" t="n">
         <v>23</v>
       </c>
     </row>
@@ -8963,7 +9147,7 @@
       <c r="C1000" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N101">
+  <autoFilter ref="A1:O101">
     <filterColumn colId="8">
       <filters>
         <filter val="SI"/>
@@ -8996,7 +9180,7 @@
       <selection pane="bottomRight" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.8125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="2" style="0" width="10.86"/>
@@ -9007,133 +9191,133 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="Q1" s="21" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="V1" s="21" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="X1" s="21" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="Y1" s="21" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="Z1" s="21" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="AA1" s="21" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="AB1" s="21" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="AC1" s="21" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="AD1" s="21" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="AE1" s="21" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="AF1" s="21" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="AG1" s="21" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="AH1" s="22" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="AI1" s="21" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="AJ1" s="21" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="AK1" s="21" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="AL1" s="21" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="AM1" s="21" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="AN1" s="23" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="AO1" s="23" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="AP1" s="4" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="AQ1" s="24" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="AR1" s="24" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23458,18 +23642,18 @@
       <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="0" t="n">
         <f aca="false">COUNTIF(CONC!I:I,A1)+COUNTIF(CONC!I:I,"chek")</f>
         <v>56</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="F1" s="0" t="n">
         <f aca="false">B1</f>
@@ -23478,7 +23662,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">COUNTIF(CONC!I:I,A2)</f>
@@ -23494,14 +23678,14 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">COUNTIF(CONC!I:I,A3)</f>
         <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="0" t="n">
         <f aca="false">COUNTIF(CONC!J2:J105,"Regional")</f>
@@ -23510,14 +23694,14 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">COUNTIF(CONC!I:I,A4)</f>
         <v>4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">B5+B6</f>
@@ -23526,14 +23710,14 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">COUNTIF(CONC!I:I,A5)</f>
         <v>23</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="F5" s="0" t="n">
         <f aca="false">B7+B4+B9</f>
@@ -23542,14 +23726,14 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">COUNTIF(CONC!I:I,A6)</f>
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="F6" s="0" t="n">
         <f aca="false">B2+B3</f>
@@ -23558,7 +23742,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">COUNTIF(CONC!I:I,A7)</f>
@@ -23567,7 +23751,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="0" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">F7+F6+F5</f>
@@ -23576,7 +23760,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">COUNTIF(CONC!I:I,A9)</f>
@@ -23585,7 +23769,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">SUM(B1:B12)</f>
@@ -23594,7 +23778,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B16" s="0" t="n">
         <f aca="false">B9+B7+B4+B3+B2</f>

</xml_diff>